<commit_message>
implemented dotted/dotless i feature
</commit_message>
<xml_diff>
--- a/external/languages.xlsx
+++ b/external/languages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\layout\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FC933-11E2-4242-B451-DBA45525852F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BFCA31-C49D-43E7-B78A-7ED5FECF8AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="330" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
@@ -3924,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H217"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6940,9 +6940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD1639C-385C-47BC-8A27-65B4241092EB}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10180,9 +10178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B12BA8A-8033-48C5-82D9-E4D112EC98EE}">
   <dimension ref="A1:U190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
realized 'gk' and 'жчщ' replace, added this to images/sheets; upd readme
</commit_message>
<xml_diff>
--- a/external/languages.xlsx
+++ b/external/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\layout\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F171510C-F4CC-46A4-9F37-F06C96CEF7F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E09623-1661-4BE6-9DD7-D22EFAE4E320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,17 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="954">
   <si>
     <t>English</t>
   </si>
@@ -3164,10 +3159,13 @@
     </r>
   </si>
   <si>
-    <t>* 10 September 2021</t>
-  </si>
-  <si>
     <t>[1] (values &lt; 0.0001% rounded to 0.0001%):</t>
+  </si>
+  <si>
+    <t>* 10 October 2021</t>
+  </si>
+  <si>
+    <t>Norwegian Bokmål</t>
   </si>
 </sst>
 </file>
@@ -3488,8 +3486,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3502,12 +3506,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4035,15 +4033,15 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
+        <v>951</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" t="s">
         <v>952</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4070,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="45">
-        <v>0.625</v>
+        <v>0.629</v>
       </c>
       <c r="C4" s="22">
         <v>1</v>
@@ -4081,7 +4079,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="45">
-        <v>7.4999999999999997E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="C5" s="22">
         <v>1</v>
@@ -4121,7 +4119,7 @@
       </c>
       <c r="H7" s="37">
         <f>SUMIF($C$4:$C$201, 1, $B$4:$B$201)</f>
-        <v>0.77274800000000032</v>
+        <v>0.77272800000000041</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4145,7 +4143,7 @@
       </c>
       <c r="H8" s="37">
         <f>SUMIF($C$4:$C$201, 2, $B$4:$B$201)</f>
-        <v>6.3557000000000016E-2</v>
+        <v>6.2567000000000025E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4153,7 +4151,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="45">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C9" s="22">
         <v>1</v>
@@ -4166,7 +4164,7 @@
       </c>
       <c r="H9" s="37">
         <f>SUMIF($C$4:$C$201, 3, $B$4:$B$201)</f>
-        <v>5.231400000000002E-2</v>
+        <v>5.222400000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4174,7 +4172,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="45">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C10" s="22">
         <v>2</v>
@@ -4232,7 +4230,7 @@
       </c>
       <c r="H12" s="37">
         <f>SUMIF($C$4:$C$201, 6, $B$4:$B$201)</f>
-        <v>6.1600000000000012E-4</v>
+        <v>5.9600000000000007E-4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,7 +4254,7 @@
       </c>
       <c r="H13" s="37">
         <f>SUMIF($C$4:$C$201, 7, $B$4:$B$201)</f>
-        <v>0.10184800000000001</v>
+        <v>0.10091800000000001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4280,7 +4278,7 @@
       </c>
       <c r="H14" s="37">
         <f>SUMIF($C$4:$C$201, 8, $B$4:$B$201)</f>
-        <v>2.8800000000000022E-4</v>
+        <v>2.980000000000002E-4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4288,7 +4286,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="45">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C15" s="22">
         <v>1</v>
@@ -4331,16 +4329,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="45">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C18" s="33">
-        <v>7</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>180</v>
+      <c r="C18" s="22">
+        <v>3</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>828</v>
       </c>
       <c r="G18" t="s">
         <v>837</v>
@@ -4348,16 +4346,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="45">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C19" s="22">
-        <v>3</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>828</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="56">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="G19" t="s">
         <v>834</v>
@@ -4600,7 +4598,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>33</v>
+        <v>953</v>
       </c>
       <c r="B37" s="45">
         <v>1E-3</v>
@@ -4618,8 +4616,8 @@
       <c r="A39" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="63">
-        <v>5.0000000000000001E-4</v>
+      <c r="B39" s="58">
+        <v>4.8000000000000001E-4</v>
       </c>
       <c r="C39" s="22">
         <v>6</v>
@@ -4632,8 +4630,8 @@
       <c r="A40" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="63">
-        <v>5.0000000000000001E-4</v>
+      <c r="B40" s="58">
+        <v>4.4999999999999999E-4</v>
       </c>
       <c r="C40" s="22">
         <v>3</v>
@@ -4644,35 +4642,35 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="63">
-        <v>4.0000000000000002E-4</v>
+        <v>33</v>
+      </c>
+      <c r="B41" s="58">
+        <v>4.0999999999999999E-4</v>
       </c>
       <c r="C41" s="22">
-        <v>4</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>701</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="63">
+        <v>41</v>
+      </c>
+      <c r="B42" s="58">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C42" s="22">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="63">
-        <v>4.0000000000000002E-4</v>
+      <c r="B43" s="58">
+        <v>3.6999999999999999E-4</v>
       </c>
       <c r="C43" s="22">
         <v>3</v>
@@ -4685,8 +4683,8 @@
       <c r="A44" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="63">
-        <v>4.0000000000000002E-4</v>
+      <c r="B44" s="58">
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="C44" s="22">
         <v>1</v>
@@ -4696,8 +4694,8 @@
       <c r="A45" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="63">
-        <v>4.0000000000000002E-4</v>
+      <c r="B45" s="58">
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="C45" s="22">
         <v>3</v>
@@ -4710,8 +4708,8 @@
       <c r="A46" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="63">
-        <v>2.9999999999999997E-4</v>
+      <c r="B46" s="58">
+        <v>3.5E-4</v>
       </c>
       <c r="C46" s="33">
         <v>7</v>
@@ -4724,8 +4722,8 @@
       <c r="A47" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="63">
-        <v>2.9999999999999997E-4</v>
+      <c r="B47" s="58">
+        <v>3.1E-4</v>
       </c>
       <c r="C47" s="22">
         <v>3</v>
@@ -4738,8 +4736,8 @@
       <c r="A48" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="63">
-        <v>2.0000000000000001E-4</v>
+      <c r="B48" s="58">
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="C48" s="22">
         <v>3</v>
@@ -4752,8 +4750,8 @@
       <c r="A49" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="63">
-        <v>2.0000000000000001E-4</v>
+      <c r="B49" s="58">
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="C49" s="22">
         <v>1</v>
@@ -4763,8 +4761,8 @@
       <c r="A50" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="63">
-        <v>2.0000000000000001E-4</v>
+      <c r="B50" s="58">
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="C50" s="33">
         <v>7</v>
@@ -4777,7 +4775,7 @@
       <c r="A51" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="63">
+      <c r="B51" s="58">
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="C51" s="33">
@@ -4791,7 +4789,7 @@
       <c r="A52" s="33" t="s">
         <v>841</v>
       </c>
-      <c r="B52" s="64">
+      <c r="B52" s="60">
         <v>1.7000000000000001E-4</v>
       </c>
       <c r="C52" s="22" t="s">
@@ -4805,7 +4803,7 @@
       <c r="A53" s="33" t="s">
         <v>842</v>
       </c>
-      <c r="B53" s="64"/>
+      <c r="B53" s="60"/>
       <c r="C53" s="22">
         <v>3</v>
       </c>
@@ -4817,7 +4815,7 @@
       <c r="A54" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="63">
+      <c r="B54" s="58">
         <v>1.2E-4</v>
       </c>
       <c r="C54" s="22" t="s">
@@ -4831,7 +4829,7 @@
       <c r="A55" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="63">
+      <c r="B55" s="58">
         <v>1.2E-4</v>
       </c>
       <c r="C55" s="22">
@@ -4845,7 +4843,7 @@
       <c r="A56" s="33" t="s">
         <v>623</v>
       </c>
-      <c r="B56" s="64">
+      <c r="B56" s="60">
         <v>1.2E-4</v>
       </c>
       <c r="C56" s="22">
@@ -4856,7 +4854,7 @@
       <c r="A57" s="33" t="s">
         <v>624</v>
       </c>
-      <c r="B57" s="64"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="22">
         <v>3</v>
       </c>
@@ -4868,8 +4866,8 @@
       <c r="A58" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="63">
-        <v>1E-4</v>
+      <c r="B58" s="58">
+        <v>1.1E-4</v>
       </c>
       <c r="C58" s="33">
         <v>8</v>
@@ -4885,7 +4883,7 @@
       <c r="A59" s="33" t="s">
         <v>626</v>
       </c>
-      <c r="B59" s="63">
+      <c r="B59" s="58">
         <v>1E-4</v>
       </c>
       <c r="C59" s="22">
@@ -4899,7 +4897,7 @@
       <c r="A60" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="63">
+      <c r="B60" s="58">
         <v>6.9999999999999994E-5</v>
       </c>
       <c r="C60" s="22">
@@ -4913,7 +4911,7 @@
       <c r="A61" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="63">
+      <c r="B61" s="58">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C61" s="22">
@@ -4927,7 +4925,7 @@
       <c r="A62" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="63">
+      <c r="B62" s="58">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C62" s="22">
@@ -4939,7 +4937,7 @@
       <c r="A63" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="63">
+      <c r="B63" s="58">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C63" s="33">
@@ -4953,7 +4951,7 @@
       <c r="A64" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="63">
+      <c r="B64" s="58">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="C64" s="33">
@@ -4967,7 +4965,7 @@
       <c r="A65" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="63">
+      <c r="B65" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C65" s="22">
@@ -4981,7 +4979,7 @@
       <c r="A66" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="63">
+      <c r="B66" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C66" s="33">
@@ -4995,7 +4993,7 @@
       <c r="A67" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="63">
+      <c r="B67" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C67" s="33">
@@ -5009,7 +5007,7 @@
       <c r="A68" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="63">
+      <c r="B68" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C68" s="22">
@@ -5021,7 +5019,7 @@
       <c r="A69" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="63">
+      <c r="B69" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C69" s="22">
@@ -5032,7 +5030,7 @@
       <c r="A70" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="63">
+      <c r="B70" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C70" s="22">
@@ -5043,7 +5041,7 @@
       <c r="A71" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="63">
+      <c r="B71" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C71" s="33">
@@ -5057,7 +5055,7 @@
       <c r="A72" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B72" s="63">
+      <c r="B72" s="58">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="C72" s="22" t="s">
@@ -5071,7 +5069,7 @@
       <c r="A73" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="63">
+      <c r="B73" s="58">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C73" s="22">
@@ -5083,7 +5081,7 @@
       <c r="A74" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="63">
+      <c r="B74" s="58">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C74" s="22">
@@ -5094,7 +5092,7 @@
       <c r="A75" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B75" s="63">
+      <c r="B75" s="58">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C75" s="22">
@@ -5108,7 +5106,7 @@
       <c r="A76" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B76" s="63">
+      <c r="B76" s="58">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C76" s="33">
@@ -5270,7 +5268,7 @@
       <c r="A88" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="B88" s="59">
+      <c r="B88" s="61">
         <v>1.2999999999999999E-5</v>
       </c>
       <c r="C88" s="22" t="s">
@@ -5284,7 +5282,7 @@
       <c r="A89" s="33" t="s">
         <v>632</v>
       </c>
-      <c r="B89" s="59"/>
+      <c r="B89" s="61"/>
       <c r="C89" s="22">
         <v>3</v>
       </c>
@@ -5552,7 +5550,7 @@
       <c r="A110" s="33" t="s">
         <v>645</v>
       </c>
-      <c r="B110" s="59">
+      <c r="B110" s="61">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="C110" s="22">
@@ -5566,7 +5564,7 @@
       <c r="A111" s="33" t="s">
         <v>646</v>
       </c>
-      <c r="B111" s="59"/>
+      <c r="B111" s="61"/>
       <c r="C111" s="33">
         <v>9</v>
       </c>
@@ -5920,7 +5918,7 @@
       <c r="A140" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B140" s="59">
+      <c r="B140" s="61">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C140" s="33">
@@ -5934,7 +5932,7 @@
       <c r="A141" s="33" t="s">
         <v>666</v>
       </c>
-      <c r="B141" s="59"/>
+      <c r="B141" s="61"/>
       <c r="C141" s="22">
         <v>1</v>
       </c>
@@ -6026,7 +6024,7 @@
       <c r="A149" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B149" s="59">
+      <c r="B149" s="61">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C149" s="22">
@@ -6037,7 +6035,7 @@
       <c r="A150" s="33" t="s">
         <v>670</v>
       </c>
-      <c r="B150" s="59"/>
+      <c r="B150" s="61"/>
       <c r="C150" s="22">
         <v>3</v>
       </c>
@@ -6049,7 +6047,7 @@
       <c r="A151" s="33" t="s">
         <v>671</v>
       </c>
-      <c r="B151" s="59">
+      <c r="B151" s="61">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C151" s="22">
@@ -6063,7 +6061,7 @@
       <c r="A152" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="B152" s="59"/>
+      <c r="B152" s="61"/>
       <c r="C152" s="22">
         <v>6</v>
       </c>
@@ -6122,7 +6120,7 @@
       <c r="A157" s="33" t="s">
         <v>674</v>
       </c>
-      <c r="B157" s="59">
+      <c r="B157" s="61">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C157" s="22">
@@ -6136,7 +6134,7 @@
       <c r="A158" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="B158" s="59"/>
+      <c r="B158" s="61"/>
       <c r="C158" s="33">
         <v>9</v>
       </c>
@@ -6148,7 +6146,7 @@
       <c r="A159" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="B159" s="59"/>
+      <c r="B159" s="61"/>
       <c r="C159" s="22">
         <v>1</v>
       </c>
@@ -6157,7 +6155,7 @@
       <c r="A160" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="B160" s="59"/>
+      <c r="B160" s="61"/>
       <c r="C160" s="22">
         <v>3</v>
       </c>
@@ -6169,7 +6167,7 @@
       <c r="A161" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="B161" s="59"/>
+      <c r="B161" s="61"/>
       <c r="C161" s="22">
         <v>3</v>
       </c>
@@ -6181,7 +6179,7 @@
       <c r="A162" s="33" t="s">
         <v>677</v>
       </c>
-      <c r="B162" s="59"/>
+      <c r="B162" s="61"/>
       <c r="C162" s="22" t="s">
         <v>717</v>
       </c>
@@ -6193,7 +6191,7 @@
       <c r="A163" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="B163" s="59"/>
+      <c r="B163" s="61"/>
       <c r="C163" s="22">
         <v>3</v>
       </c>
@@ -6205,7 +6203,7 @@
       <c r="A164" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="B164" s="59"/>
+      <c r="B164" s="61"/>
       <c r="C164" s="22">
         <v>3</v>
       </c>
@@ -6371,7 +6369,7 @@
       <c r="A176" s="33" t="s">
         <v>688</v>
       </c>
-      <c r="B176" s="59">
+      <c r="B176" s="61">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C176" s="22" t="s">
@@ -6385,7 +6383,7 @@
       <c r="A177" s="33" t="s">
         <v>689</v>
       </c>
-      <c r="B177" s="59"/>
+      <c r="B177" s="61"/>
       <c r="C177" s="22" t="s">
         <v>729</v>
       </c>
@@ -6904,6 +6902,9 @@
       <c r="F217" s="31"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:D51">
+    <sortCondition descending="1" ref="B40:B51"/>
+  </sortState>
   <mergeCells count="10">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B52:B53"/>
@@ -8388,12 +8389,12 @@
         <v>600</v>
       </c>
       <c r="O27" s="31"/>
-      <c r="P27" s="60" t="s">
+      <c r="P27" s="62" t="s">
         <v>819</v>
       </c>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="60"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
       <c r="T27" s="31"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -9303,10 +9304,10 @@
       <c r="D17" t="s">
         <v>349</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="64">
         <v>23.6</v>
       </c>
-      <c r="G17" s="61">
+      <c r="G17" s="63">
         <v>45</v>
       </c>
     </row>
@@ -9323,8 +9324,8 @@
       <c r="D18" t="s">
         <v>478</v>
       </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="61"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="63"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -10316,10 +10317,10 @@
       <c r="E18" t="s">
         <v>765</v>
       </c>
-      <c r="F18" s="60">
+      <c r="F18" s="62">
         <v>3.5</v>
       </c>
-      <c r="G18" s="60">
+      <c r="G18" s="62">
         <v>3.5</v>
       </c>
     </row>
@@ -10333,8 +10334,8 @@
       <c r="E19" t="s">
         <v>766</v>
       </c>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">

</xml_diff>

<commit_message>
update language usage statistics
</commit_message>
<xml_diff>
--- a/external/languages.xlsx
+++ b/external/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\layout\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E09623-1661-4BE6-9DD7-D22EFAE4E320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20401A6F-E1D7-40B5-85EE-44B790060E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3162,10 +3167,10 @@
     <t>[1] (values &lt; 0.0001% rounded to 0.0001%):</t>
   </si>
   <si>
-    <t>* 10 October 2021</t>
-  </si>
-  <si>
     <t>Norwegian Bokmål</t>
+  </si>
+  <si>
+    <t>* 15 October 2021</t>
   </si>
 </sst>
 </file>
@@ -4041,7 +4046,7 @@
       <c r="C1" s="59"/>
       <c r="D1" s="59"/>
       <c r="E1" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4068,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="45">
-        <v>0.629</v>
+        <v>0.63100000000000001</v>
       </c>
       <c r="C4" s="22">
         <v>1</v>
@@ -4079,7 +4084,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="45">
-        <v>7.2999999999999995E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C5" s="22">
         <v>1</v>
@@ -4119,7 +4124,7 @@
       </c>
       <c r="H7" s="37">
         <f>SUMIF($C$4:$C$201, 1, $B$4:$B$201)</f>
-        <v>0.77272800000000041</v>
+        <v>0.77472800000000042</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4164,7 +4169,7 @@
       </c>
       <c r="H9" s="37">
         <f>SUMIF($C$4:$C$201, 3, $B$4:$B$201)</f>
-        <v>5.222400000000002E-2</v>
+        <v>5.2204000000000021E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4307,7 +4312,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="45">
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -4598,7 +4603,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B37" s="45">
         <v>1E-3</v>
@@ -4631,7 +4636,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="58">
-        <v>4.4999999999999999E-4</v>
+        <v>4.2999999999999999E-4</v>
       </c>
       <c r="C40" s="22">
         <v>3</v>
@@ -6902,7 +6907,7 @@
       <c r="F217" s="31"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:D51">
+  <sortState ref="A40:D51">
     <sortCondition descending="1" ref="B40:B51"/>
   </sortState>
   <mergeCells count="10">

</xml_diff>

<commit_message>
update language usage statistics; add cheatsheet.png
</commit_message>
<xml_diff>
--- a/external/languages.xlsx
+++ b/external/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\layout\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20401A6F-E1D7-40B5-85EE-44B790060E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32399EE-CFE0-4ED4-9B75-25DF585CB9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3170,16 +3170,17 @@
     <t>Norwegian Bokmål</t>
   </si>
   <si>
-    <t>* 15 October 2021</t>
+    <t>* 19 October 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -3342,7 +3343,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3454,9 +3455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3494,6 +3492,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4018,10 +4023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H217"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H9"/>
+      <selection activeCell="I7" sqref="I7:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4033,28 +4038,29 @@
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>951</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>38</v>
       </c>
@@ -4068,22 +4074,22 @@
         <v>628</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="59">
         <v>0.63100000000000001</v>
       </c>
       <c r="C4" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="59">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="C5" s="22">
@@ -4091,11 +4097,11 @@
       </c>
       <c r="H5" s="33"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="59">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="C6" s="22">
@@ -4106,11 +4112,11 @@
       </c>
       <c r="H6" s="38"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="59">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="C7" s="22">
@@ -4124,14 +4130,18 @@
       </c>
       <c r="H7" s="37">
         <f>SUMIF($C$4:$C$201, 1, $B$4:$B$201)</f>
-        <v>0.77472800000000042</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.77472600000000058</v>
+      </c>
+      <c r="I7" s="60">
+        <f>H7/SUM($H$7:$H$15)</f>
+        <v>0.77419722329648877</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="59">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C8" s="22">
@@ -4148,14 +4158,18 @@
       </c>
       <c r="H8" s="37">
         <f>SUMIF($C$4:$C$201, 2, $B$4:$B$201)</f>
-        <v>6.2567000000000025E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.2573999999999991E-2</v>
+      </c>
+      <c r="I8" s="60">
+        <f t="shared" ref="I8:I15" si="0">H8/SUM($H$7:$H$15)</f>
+        <v>6.253129112815943E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="59">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C9" s="22">
@@ -4169,14 +4183,18 @@
       </c>
       <c r="H9" s="37">
         <f>SUMIF($C$4:$C$201, 3, $B$4:$B$201)</f>
-        <v>5.2204000000000021E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.2165000000000024E-2</v>
+      </c>
+      <c r="I9" s="60">
+        <f t="shared" si="0"/>
+        <v>5.2129395622789634E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="59">
         <v>0.02</v>
       </c>
       <c r="C10" s="22">
@@ -4192,12 +4210,16 @@
         <f>SUMIF($C$4:$C$201, 4, $B$4:$B$201)</f>
         <v>7.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="60">
+        <f t="shared" si="0"/>
+        <v>7.3949492496624778E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="59">
         <v>1.9E-2</v>
       </c>
       <c r="C11" s="22">
@@ -4216,12 +4238,16 @@
         <f>SUMIF($C$4:$C$201, 5, $B$4:$B$201)</f>
         <v>3.0030000000000005E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="60">
+        <f t="shared" si="0"/>
+        <v>3.0009503509103273E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="59">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C12" s="22">
@@ -4235,14 +4261,18 @@
       </c>
       <c r="H12" s="37">
         <f>SUMIF($C$4:$C$201, 6, $B$4:$B$201)</f>
-        <v>5.9600000000000007E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.8600000000000026E-4</v>
+      </c>
+      <c r="I12" s="60">
+        <f t="shared" si="0"/>
+        <v>5.8560003517597479E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="59">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="C13" s="22">
@@ -4259,14 +4289,18 @@
       </c>
       <c r="H13" s="37">
         <f>SUMIF($C$4:$C$201, 7, $B$4:$B$201)</f>
-        <v>0.10091800000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9.9926000000000015E-2</v>
+      </c>
+      <c r="I13" s="60">
+        <f t="shared" si="0"/>
+        <v>9.9857797124563899E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="59">
         <v>1.2E-2</v>
       </c>
       <c r="C14" s="22">
@@ -4283,15 +4317,19 @@
       </c>
       <c r="H14" s="37">
         <f>SUMIF($C$4:$C$201, 8, $B$4:$B$201)</f>
-        <v>2.980000000000002E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.9500000000000018E-4</v>
+      </c>
+      <c r="I14" s="60">
+        <f t="shared" si="0"/>
+        <v>2.9479865252032866E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="45">
-        <v>7.0000000000000001E-3</v>
+        <v>12</v>
+      </c>
+      <c r="B15" s="59">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C15" s="22">
         <v>1</v>
@@ -4306,13 +4344,17 @@
         <f>SUMIF($C$4:$C$201, 9, $B$4:$B$201)</f>
         <v>7.9999999999999996E-6</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="60">
+        <f t="shared" si="0"/>
+        <v>7.9945397293648407E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="45">
-        <v>8.0000000000000002E-3</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="59">
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C16" s="22">
         <v>1</v>
@@ -4322,7 +4364,7 @@
       <c r="A17" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="59">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="C17" s="22">
@@ -4336,7 +4378,7 @@
       <c r="A18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="59">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C18" s="22">
@@ -4351,16 +4393,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="45">
+        <v>16</v>
+      </c>
+      <c r="B19" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C19" s="56">
-        <v>7</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>180</v>
+      <c r="C19" s="22">
+        <v>1</v>
       </c>
       <c r="G19" t="s">
         <v>834</v>
@@ -4368,13 +4407,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="45">
+        <v>17</v>
+      </c>
+      <c r="B20" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C20" s="22">
-        <v>1</v>
+      <c r="C20" s="55">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="G20" t="s">
         <v>835</v>
@@ -4382,16 +4424,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="45">
+        <v>19</v>
+      </c>
+      <c r="B21" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C21" s="33">
         <v>7</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G21" t="s">
         <v>836</v>
@@ -4399,16 +4441,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="45">
+        <v>18</v>
+      </c>
+      <c r="B22" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C22" s="33">
         <v>7</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G22" t="s">
         <v>838</v>
@@ -4416,16 +4458,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="45">
+        <v>20</v>
+      </c>
+      <c r="B23" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C23" s="33">
-        <v>7</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>178</v>
+      <c r="C23" s="22">
+        <v>4</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>722</v>
       </c>
       <c r="G23" t="s">
         <v>910</v>
@@ -4433,23 +4475,23 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="45">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C24" s="22">
-        <v>4</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>722</v>
+        <v>14</v>
+      </c>
+      <c r="B24" s="59">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="55">
+        <v>7</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B25" s="59">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C25" s="22">
@@ -4463,7 +4505,7 @@
       <c r="A26" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="59">
         <v>2E-3</v>
       </c>
       <c r="C26" s="22">
@@ -4477,7 +4519,7 @@
       <c r="A27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B27" s="59">
         <v>2E-3</v>
       </c>
       <c r="C27" s="22">
@@ -4488,7 +4530,7 @@
       <c r="A28" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="59">
         <v>2E-3</v>
       </c>
       <c r="C28" s="22">
@@ -4502,7 +4544,7 @@
       <c r="A29" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B29" s="59">
         <v>1E-3</v>
       </c>
       <c r="C29" s="22">
@@ -4516,7 +4558,7 @@
       <c r="A30" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="45">
+      <c r="B30" s="59">
         <v>1E-3</v>
       </c>
       <c r="C30" s="22">
@@ -4527,7 +4569,7 @@
       <c r="A31" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="45">
+      <c r="B31" s="59">
         <v>1E-3</v>
       </c>
       <c r="C31" s="22">
@@ -4538,7 +4580,7 @@
       <c r="A32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="59">
         <v>1E-3</v>
       </c>
       <c r="C32" s="22">
@@ -4549,7 +4591,7 @@
       <c r="A33" s="33" t="s">
         <v>709</v>
       </c>
-      <c r="B33" s="45">
+      <c r="B33" s="59">
         <v>1E-3</v>
       </c>
       <c r="C33" s="22">
@@ -4563,7 +4605,7 @@
       <c r="A34" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="45">
+      <c r="B34" s="59">
         <v>1E-3</v>
       </c>
       <c r="C34" s="22">
@@ -4577,7 +4619,7 @@
       <c r="A35" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="45">
+      <c r="B35" s="59">
         <v>1E-3</v>
       </c>
       <c r="C35" s="33">
@@ -4591,7 +4633,7 @@
       <c r="A36" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="59">
         <v>1E-3</v>
       </c>
       <c r="C36" s="22">
@@ -4605,7 +4647,7 @@
       <c r="A37" s="33" t="s">
         <v>952</v>
       </c>
-      <c r="B37" s="45">
+      <c r="B37" s="59">
         <v>1E-3</v>
       </c>
       <c r="C37" s="22">
@@ -4621,8 +4663,8 @@
       <c r="A39" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="58">
-        <v>4.8000000000000001E-4</v>
+      <c r="B39" s="57">
+        <v>4.6999999999999999E-4</v>
       </c>
       <c r="C39" s="22">
         <v>6</v>
@@ -4635,7 +4677,7 @@
       <c r="A40" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="58">
+      <c r="B40" s="57">
         <v>4.2999999999999999E-4</v>
       </c>
       <c r="C40" s="22">
@@ -4649,8 +4691,8 @@
       <c r="A41" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="58">
-        <v>4.0999999999999999E-4</v>
+      <c r="B41" s="57">
+        <v>4.2000000000000002E-4</v>
       </c>
       <c r="C41" s="22">
         <v>2</v>
@@ -4660,7 +4702,7 @@
       <c r="A42" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="58">
+      <c r="B42" s="57">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C42" s="22">
@@ -4674,8 +4716,8 @@
       <c r="A43" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="58">
-        <v>3.6999999999999999E-4</v>
+      <c r="B43" s="57">
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="C43" s="22">
         <v>3</v>
@@ -4688,7 +4730,7 @@
       <c r="A44" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="58">
+      <c r="B44" s="57">
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="C44" s="22">
@@ -4699,8 +4741,8 @@
       <c r="A45" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="58">
-        <v>3.6000000000000002E-4</v>
+      <c r="B45" s="57">
+        <v>3.5E-4</v>
       </c>
       <c r="C45" s="22">
         <v>3</v>
@@ -4713,7 +4755,7 @@
       <c r="A46" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="58">
+      <c r="B46" s="57">
         <v>3.5E-4</v>
       </c>
       <c r="C46" s="33">
@@ -4727,8 +4769,8 @@
       <c r="A47" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="58">
-        <v>3.1E-4</v>
+      <c r="B47" s="57">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="C47" s="22">
         <v>3</v>
@@ -4738,10 +4780,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="58">
+      <c r="B48" s="57">
         <v>2.2000000000000001E-4</v>
       </c>
       <c r="C48" s="22">
@@ -4752,10 +4794,10 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="58">
+      <c r="B49" s="57">
         <v>2.2000000000000001E-4</v>
       </c>
       <c r="C49" s="22">
@@ -4766,8 +4808,8 @@
       <c r="A50" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="58">
-        <v>2.2000000000000001E-4</v>
+      <c r="B50" s="57">
+        <v>2.3000000000000001E-4</v>
       </c>
       <c r="C50" s="33">
         <v>7</v>
@@ -4780,7 +4822,7 @@
       <c r="A51" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="58">
+      <c r="B51" s="57">
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="C51" s="33">
@@ -4794,8 +4836,8 @@
       <c r="A52" s="33" t="s">
         <v>841</v>
       </c>
-      <c r="B52" s="60">
-        <v>1.7000000000000001E-4</v>
+      <c r="B52" s="62">
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>729</v>
@@ -4808,7 +4850,7 @@
       <c r="A53" s="33" t="s">
         <v>842</v>
       </c>
-      <c r="B53" s="60"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="22">
         <v>3</v>
       </c>
@@ -4820,7 +4862,7 @@
       <c r="A54" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="58">
+      <c r="B54" s="57">
         <v>1.2E-4</v>
       </c>
       <c r="C54" s="22" t="s">
@@ -4834,7 +4876,7 @@
       <c r="A55" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="58">
+      <c r="B55" s="57">
         <v>1.2E-4</v>
       </c>
       <c r="C55" s="22">
@@ -4848,7 +4890,7 @@
       <c r="A56" s="33" t="s">
         <v>623</v>
       </c>
-      <c r="B56" s="60">
+      <c r="B56" s="62">
         <v>1.2E-4</v>
       </c>
       <c r="C56" s="22">
@@ -4859,7 +4901,7 @@
       <c r="A57" s="33" t="s">
         <v>624</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="62"/>
       <c r="C57" s="22">
         <v>3</v>
       </c>
@@ -4871,13 +4913,13 @@
       <c r="A58" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="58">
+      <c r="B58" s="57">
         <v>1.1E-4</v>
       </c>
       <c r="C58" s="33">
         <v>8</v>
       </c>
-      <c r="D58" s="48" t="s">
+      <c r="D58" s="47" t="s">
         <v>867</v>
       </c>
       <c r="E58" s="24" t="s">
@@ -4888,7 +4930,7 @@
       <c r="A59" s="33" t="s">
         <v>626</v>
       </c>
-      <c r="B59" s="58">
+      <c r="B59" s="57">
         <v>1E-4</v>
       </c>
       <c r="C59" s="22">
@@ -4903,7 +4945,7 @@
         <v>55</v>
       </c>
       <c r="B60" s="58">
-        <v>6.9999999999999994E-5</v>
+        <v>6.4999999999999994E-5</v>
       </c>
       <c r="C60" s="22">
         <v>3</v>
@@ -4917,7 +4959,7 @@
         <v>56</v>
       </c>
       <c r="B61" s="58">
-        <v>5.0000000000000002E-5</v>
+        <v>5.1999999999999997E-5</v>
       </c>
       <c r="C61" s="22">
         <v>6</v>
@@ -4931,7 +4973,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="58">
-        <v>5.0000000000000002E-5</v>
+        <v>4.8999999999999998E-5</v>
       </c>
       <c r="C62" s="22">
         <v>2</v>
@@ -4943,7 +4985,7 @@
         <v>57</v>
       </c>
       <c r="B63" s="58">
-        <v>5.0000000000000002E-5</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="C63" s="33">
         <v>7</v>
@@ -4957,7 +4999,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="58">
-        <v>4.0000000000000003E-5</v>
+        <v>4.1E-5</v>
       </c>
       <c r="C64" s="33">
         <v>7</v>
@@ -5025,7 +5067,7 @@
         <v>64</v>
       </c>
       <c r="B69" s="58">
-        <v>3.0000000000000001E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="C69" s="22">
         <v>2</v>
@@ -5036,7 +5078,7 @@
         <v>65</v>
       </c>
       <c r="B70" s="58">
-        <v>3.0000000000000001E-5</v>
+        <v>2.8E-5</v>
       </c>
       <c r="C70" s="22">
         <v>2</v>
@@ -5047,7 +5089,7 @@
         <v>66</v>
       </c>
       <c r="B71" s="58">
-        <v>3.0000000000000001E-5</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="C71" s="33">
         <v>8</v>
@@ -5061,7 +5103,7 @@
         <v>67</v>
       </c>
       <c r="B72" s="58">
-        <v>3.0000000000000001E-5</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="C72" s="22" t="s">
         <v>859</v>
@@ -5075,7 +5117,7 @@
         <v>69</v>
       </c>
       <c r="B73" s="58">
-        <v>2.0000000000000002E-5</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="C73" s="22">
         <v>2</v>
@@ -5087,7 +5129,7 @@
         <v>68</v>
       </c>
       <c r="B74" s="58">
-        <v>2.0000000000000002E-5</v>
+        <v>2.0999999999999999E-5</v>
       </c>
       <c r="C74" s="22">
         <v>2</v>
@@ -5112,7 +5154,7 @@
         <v>71</v>
       </c>
       <c r="B76" s="58">
-        <v>2.0000000000000002E-5</v>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="C76" s="33">
         <v>8</v>
@@ -5125,7 +5167,7 @@
       <c r="A77" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="57">
+      <c r="B77" s="56">
         <v>1.8E-5</v>
       </c>
       <c r="C77" s="33">
@@ -5139,8 +5181,8 @@
       <c r="A78" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="57">
-        <v>1.7E-5</v>
+      <c r="B78" s="56">
+        <v>1.5E-5</v>
       </c>
       <c r="C78" s="33">
         <v>8</v>
@@ -5153,8 +5195,8 @@
       <c r="A79" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="57">
-        <v>1.7E-5</v>
+      <c r="B79" s="56">
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="C79" s="33">
         <v>8</v>
@@ -5167,8 +5209,8 @@
       <c r="A80" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="57">
-        <v>1.7E-5</v>
+      <c r="B80" s="56">
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="C80" s="22">
         <v>1</v>
@@ -5178,7 +5220,7 @@
       <c r="A81" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B81" s="57">
+      <c r="B81" s="56">
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="C81" s="33">
@@ -5192,8 +5234,8 @@
       <c r="A82" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B82" s="57">
-        <v>1.5E-5</v>
+      <c r="B82" s="56">
+        <v>1.4E-5</v>
       </c>
       <c r="C82" s="22">
         <v>3</v>
@@ -5206,8 +5248,8 @@
       <c r="A83" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="57">
-        <v>1.4E-5</v>
+      <c r="B83" s="56">
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="C83" s="33">
         <v>7</v>
@@ -5220,8 +5262,8 @@
       <c r="A84" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="57">
-        <v>1.4E-5</v>
+      <c r="B84" s="56">
+        <v>1.2E-5</v>
       </c>
       <c r="C84" s="22">
         <v>1</v>
@@ -5231,8 +5273,8 @@
       <c r="A85" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="57">
-        <v>1.4E-5</v>
+      <c r="B85" s="56">
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="C85" s="22">
         <v>3</v>
@@ -5245,7 +5287,7 @@
       <c r="A86" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B86" s="57">
+      <c r="B86" s="56">
         <v>1.2999999999999999E-5</v>
       </c>
       <c r="C86" s="33">
@@ -5259,7 +5301,7 @@
       <c r="A87" s="33" t="s">
         <v>634</v>
       </c>
-      <c r="B87" s="57">
+      <c r="B87" s="56">
         <v>1.2999999999999999E-5</v>
       </c>
       <c r="C87" s="22">
@@ -5273,8 +5315,8 @@
       <c r="A88" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="B88" s="61">
-        <v>1.2999999999999999E-5</v>
+      <c r="B88" s="63">
+        <v>1.2E-5</v>
       </c>
       <c r="C88" s="22" t="s">
         <v>717</v>
@@ -5287,7 +5329,7 @@
       <c r="A89" s="33" t="s">
         <v>632</v>
       </c>
-      <c r="B89" s="61"/>
+      <c r="B89" s="63"/>
       <c r="C89" s="22">
         <v>3</v>
       </c>
@@ -5299,8 +5341,8 @@
       <c r="A90" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B90" s="57">
-        <v>1.1E-5</v>
+      <c r="B90" s="56">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C90" s="22">
         <v>3</v>
@@ -5313,7 +5355,7 @@
       <c r="A91" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="57">
+      <c r="B91" s="56">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C91" s="22" t="s">
@@ -5327,8 +5369,8 @@
       <c r="A92" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="B92" s="57">
-        <v>1.0000000000000001E-5</v>
+      <c r="B92" s="56">
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="C92" s="22">
         <v>1</v>
@@ -5338,8 +5380,8 @@
       <c r="A93" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="57">
-        <v>1.0000000000000001E-5</v>
+      <c r="B93" s="56">
+        <v>1.1E-5</v>
       </c>
       <c r="C93" s="22">
         <v>3</v>
@@ -5352,7 +5394,7 @@
       <c r="A94" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B94" s="57">
+      <c r="B94" s="56">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C94" s="33">
@@ -5366,7 +5408,7 @@
       <c r="A95" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B95" s="57">
+      <c r="B95" s="56">
         <v>9.0000000000000002E-6</v>
       </c>
       <c r="C95" s="33">
@@ -5380,8 +5422,8 @@
       <c r="A96" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B96" s="57">
-        <v>7.9999999999999996E-6</v>
+      <c r="B96" s="56">
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="C96" s="33">
         <v>7</v>
@@ -5394,8 +5436,8 @@
       <c r="A97" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B97" s="57">
-        <v>7.9999999999999996E-6</v>
+      <c r="B97" s="56">
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="C97" s="22">
         <v>3</v>
@@ -5408,7 +5450,7 @@
       <c r="A98" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B98" s="57">
+      <c r="B98" s="56">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="C98" s="33">
@@ -5419,7 +5461,7 @@
       <c r="A99" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B99" s="57">
+      <c r="B99" s="56">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="C99" s="22">
@@ -5430,7 +5472,7 @@
       <c r="A100" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B100" s="57">
+      <c r="B100" s="56">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="C100" s="22">
@@ -5441,7 +5483,7 @@
       <c r="A101" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B101" s="57">
+      <c r="B101" s="56">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="C101" s="22">
@@ -5455,7 +5497,7 @@
       <c r="A102" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B102" s="57">
+      <c r="B102" s="56">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="C102" s="22">
@@ -5466,7 +5508,7 @@
       <c r="A103" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="B103" s="57">
+      <c r="B103" s="56">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="C103" s="33">
@@ -5480,8 +5522,8 @@
       <c r="A104" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B104" s="57">
-        <v>6.9999999999999999E-6</v>
+      <c r="B104" s="56">
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="C104" s="22">
         <v>1</v>
@@ -5491,8 +5533,8 @@
       <c r="A105" s="33" t="s">
         <v>644</v>
       </c>
-      <c r="B105" s="57">
-        <v>6.9999999999999999E-6</v>
+      <c r="B105" s="56">
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="C105" s="22">
         <v>1</v>
@@ -5502,7 +5544,7 @@
       <c r="A106" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B106" s="57">
+      <c r="B106" s="56">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="C106" s="22">
@@ -5513,7 +5555,7 @@
       <c r="A107" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B107" s="57">
+      <c r="B107" s="56">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="C107" s="33">
@@ -5527,7 +5569,7 @@
       <c r="A108" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B108" s="57">
+      <c r="B108" s="56">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="C108" s="22">
@@ -5541,7 +5583,7 @@
       <c r="A109" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="57">
+      <c r="B109" s="56">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="C109" s="22">
@@ -5555,7 +5597,7 @@
       <c r="A110" s="33" t="s">
         <v>645</v>
       </c>
-      <c r="B110" s="61">
+      <c r="B110" s="63">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="C110" s="22">
@@ -5569,7 +5611,7 @@
       <c r="A111" s="33" t="s">
         <v>646</v>
       </c>
-      <c r="B111" s="61"/>
+      <c r="B111" s="63"/>
       <c r="C111" s="33">
         <v>9</v>
       </c>
@@ -5579,8 +5621,8 @@
       <c r="A112" s="33" t="s">
         <v>647</v>
       </c>
-      <c r="B112" s="57">
-        <v>3.0000000000000001E-6</v>
+      <c r="B112" s="56">
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="C112" s="22">
         <v>6</v>
@@ -5593,7 +5635,7 @@
       <c r="A113" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B113" s="57">
+      <c r="B113" s="56">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="C113" s="22">
@@ -5604,7 +5646,7 @@
       <c r="A114" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B114" s="57">
+      <c r="B114" s="56">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="C114" s="33">
@@ -5618,8 +5660,8 @@
       <c r="A115" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="B115" s="57">
-        <v>3.0000000000000001E-6</v>
+      <c r="B115" s="56">
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="C115" s="22">
         <v>6</v>
@@ -5632,8 +5674,8 @@
       <c r="A116" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="B116" s="57">
-        <v>1.9999999999999999E-6</v>
+      <c r="B116" s="56">
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="C116" s="22">
         <v>1</v>
@@ -5643,7 +5685,7 @@
       <c r="A117" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B117" s="57">
+      <c r="B117" s="56">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="C117" s="22">
@@ -5654,7 +5696,7 @@
       <c r="A118" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B118" s="57">
+      <c r="B118" s="56">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="C118" s="22" t="s">
@@ -5668,8 +5710,8 @@
       <c r="A119" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B119" s="57">
-        <v>1.9999999999999999E-6</v>
+      <c r="B119" s="56">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C119" s="22">
         <v>3</v>
@@ -5682,7 +5724,7 @@
       <c r="A120" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="B120" s="57">
+      <c r="B120" s="56">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="C120" s="22">
@@ -5693,7 +5735,7 @@
       <c r="A121" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B121" s="57">
+      <c r="B121" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C121" s="22">
@@ -5707,7 +5749,7 @@
       <c r="A122" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="B122" s="57">
+      <c r="B122" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C122" s="22">
@@ -5718,7 +5760,7 @@
       <c r="A123" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B123" s="57">
+      <c r="B123" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C123" s="33">
@@ -5732,7 +5774,7 @@
       <c r="A124" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="B124" s="57">
+      <c r="B124" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C124" s="22">
@@ -5743,7 +5785,7 @@
       <c r="A125" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="B125" s="57">
+      <c r="B125" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C125" s="22">
@@ -5754,7 +5796,7 @@
       <c r="A126" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B126" s="57">
+      <c r="B126" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C126" s="33">
@@ -5768,8 +5810,8 @@
       <c r="A127" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B127" s="57">
-        <v>9.9999999999999995E-7</v>
+      <c r="B127" s="56">
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="C127" s="33">
         <v>8</v>
@@ -5782,7 +5824,7 @@
       <c r="A128" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="B128" s="57">
+      <c r="B128" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C128" s="22">
@@ -5793,7 +5835,7 @@
       <c r="A129" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B129" s="57">
+      <c r="B129" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C129" s="22">
@@ -5807,7 +5849,7 @@
       <c r="A130" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B130" s="57">
+      <c r="B130" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C130" s="22">
@@ -5818,7 +5860,7 @@
       <c r="A131" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B131" s="57">
+      <c r="B131" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C131" s="22">
@@ -5832,7 +5874,7 @@
       <c r="A132" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="B132" s="57">
+      <c r="B132" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C132" s="22">
@@ -5843,7 +5885,7 @@
       <c r="A133" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B133" s="57">
+      <c r="B133" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C133" s="22">
@@ -5854,7 +5896,7 @@
       <c r="A134" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B134" s="57">
+      <c r="B134" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C134" s="22">
@@ -5865,7 +5907,7 @@
       <c r="A135" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B135" s="57">
+      <c r="B135" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C135" s="22">
@@ -5876,7 +5918,7 @@
       <c r="A136" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="B136" s="57">
+      <c r="B136" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C136" s="22">
@@ -5887,7 +5929,7 @@
       <c r="A137" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B137" s="57">
+      <c r="B137" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C137" s="22">
@@ -5898,7 +5940,7 @@
       <c r="A138" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B138" s="57">
+      <c r="B138" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C138" s="33">
@@ -5912,7 +5954,7 @@
       <c r="A139" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="B139" s="57">
+      <c r="B139" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C139" s="22">
@@ -5923,7 +5965,7 @@
       <c r="A140" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B140" s="61">
+      <c r="B140" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C140" s="33">
@@ -5937,7 +5979,7 @@
       <c r="A141" s="33" t="s">
         <v>666</v>
       </c>
-      <c r="B141" s="61"/>
+      <c r="B141" s="63"/>
       <c r="C141" s="22">
         <v>1</v>
       </c>
@@ -5946,7 +5988,7 @@
       <c r="A142" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B142" s="57">
+      <c r="B142" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C142" s="22">
@@ -5957,7 +5999,7 @@
       <c r="A143" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B143" s="57">
+      <c r="B143" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C143" s="22">
@@ -5968,7 +6010,7 @@
       <c r="A144" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B144" s="57">
+      <c r="B144" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C144" s="22">
@@ -5979,7 +6021,7 @@
       <c r="A145" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B145" s="57">
+      <c r="B145" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C145" s="22">
@@ -5993,7 +6035,7 @@
       <c r="A146" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B146" s="57">
+      <c r="B146" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C146" s="22">
@@ -6007,7 +6049,7 @@
       <c r="A147" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B147" s="57">
+      <c r="B147" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C147" s="22">
@@ -6018,7 +6060,7 @@
       <c r="A148" s="33" t="s">
         <v>669</v>
       </c>
-      <c r="B148" s="57">
+      <c r="B148" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C148" s="22">
@@ -6029,7 +6071,7 @@
       <c r="A149" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B149" s="61">
+      <c r="B149" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C149" s="22">
@@ -6040,7 +6082,7 @@
       <c r="A150" s="33" t="s">
         <v>670</v>
       </c>
-      <c r="B150" s="61"/>
+      <c r="B150" s="63"/>
       <c r="C150" s="22">
         <v>3</v>
       </c>
@@ -6052,7 +6094,7 @@
       <c r="A151" s="33" t="s">
         <v>671</v>
       </c>
-      <c r="B151" s="61">
+      <c r="B151" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C151" s="22">
@@ -6066,7 +6108,7 @@
       <c r="A152" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="B152" s="61"/>
+      <c r="B152" s="63"/>
       <c r="C152" s="22">
         <v>6</v>
       </c>
@@ -6078,7 +6120,7 @@
       <c r="A153" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B153" s="57">
+      <c r="B153" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C153" s="22">
@@ -6089,7 +6131,7 @@
       <c r="A154" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="B154" s="57">
+      <c r="B154" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C154" s="22">
@@ -6100,7 +6142,7 @@
       <c r="A155" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B155" s="57">
+      <c r="B155" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C155" s="22">
@@ -6114,7 +6156,7 @@
       <c r="A156" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="B156" s="57">
+      <c r="B156" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C156" s="22">
@@ -6125,7 +6167,7 @@
       <c r="A157" s="33" t="s">
         <v>674</v>
       </c>
-      <c r="B157" s="61">
+      <c r="B157" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C157" s="22">
@@ -6139,7 +6181,7 @@
       <c r="A158" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="B158" s="61"/>
+      <c r="B158" s="63"/>
       <c r="C158" s="33">
         <v>9</v>
       </c>
@@ -6151,7 +6193,7 @@
       <c r="A159" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="B159" s="61"/>
+      <c r="B159" s="63"/>
       <c r="C159" s="22">
         <v>1</v>
       </c>
@@ -6160,7 +6202,7 @@
       <c r="A160" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="B160" s="61"/>
+      <c r="B160" s="63"/>
       <c r="C160" s="22">
         <v>3</v>
       </c>
@@ -6172,7 +6214,7 @@
       <c r="A161" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="B161" s="61"/>
+      <c r="B161" s="63"/>
       <c r="C161" s="22">
         <v>3</v>
       </c>
@@ -6184,7 +6226,7 @@
       <c r="A162" s="33" t="s">
         <v>677</v>
       </c>
-      <c r="B162" s="61"/>
+      <c r="B162" s="63"/>
       <c r="C162" s="22" t="s">
         <v>717</v>
       </c>
@@ -6196,7 +6238,7 @@
       <c r="A163" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="B163" s="61"/>
+      <c r="B163" s="63"/>
       <c r="C163" s="22">
         <v>3</v>
       </c>
@@ -6208,7 +6250,7 @@
       <c r="A164" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="B164" s="61"/>
+      <c r="B164" s="63"/>
       <c r="C164" s="22">
         <v>3</v>
       </c>
@@ -6220,10 +6262,10 @@
       <c r="A165" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B165" s="57">
+      <c r="B165" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C165" s="46" t="s">
+      <c r="C165" s="45" t="s">
         <v>727</v>
       </c>
       <c r="D165" s="25" t="s">
@@ -6237,7 +6279,7 @@
       <c r="A166" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B166" s="57">
+      <c r="B166" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C166" s="22">
@@ -6251,7 +6293,7 @@
       <c r="A167" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B167" s="57">
+      <c r="B167" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C167" s="22">
@@ -6265,7 +6307,7 @@
       <c r="A168" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B168" s="57">
+      <c r="B168" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C168" s="22">
@@ -6276,10 +6318,10 @@
       <c r="A169" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B169" s="57">
+      <c r="B169" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C169" s="47" t="s">
+      <c r="C169" s="46" t="s">
         <v>728</v>
       </c>
       <c r="D169" s="25" t="s">
@@ -6293,7 +6335,7 @@
       <c r="A170" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B170" s="57">
+      <c r="B170" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C170" s="33">
@@ -6307,7 +6349,7 @@
       <c r="A171" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B171" s="57">
+      <c r="B171" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C171" s="22">
@@ -6318,10 +6360,10 @@
       <c r="A172" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B172" s="57">
+      <c r="B172" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C172" s="47" t="s">
+      <c r="C172" s="46" t="s">
         <v>728</v>
       </c>
       <c r="D172" s="7" t="s">
@@ -6335,7 +6377,7 @@
       <c r="A173" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B173" s="57">
+      <c r="B173" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C173" s="22">
@@ -6349,7 +6391,7 @@
       <c r="A174" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B174" s="57">
+      <c r="B174" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C174" s="22">
@@ -6363,7 +6405,7 @@
       <c r="A175" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B175" s="57">
+      <c r="B175" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C175" s="22">
@@ -6374,7 +6416,7 @@
       <c r="A176" s="33" t="s">
         <v>688</v>
       </c>
-      <c r="B176" s="61">
+      <c r="B176" s="63">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C176" s="22" t="s">
@@ -6388,7 +6430,7 @@
       <c r="A177" s="33" t="s">
         <v>689</v>
       </c>
-      <c r="B177" s="61"/>
+      <c r="B177" s="63"/>
       <c r="C177" s="22" t="s">
         <v>729</v>
       </c>
@@ -6400,7 +6442,7 @@
       <c r="A178" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B178" s="57">
+      <c r="B178" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C178" s="22">
@@ -6414,7 +6456,7 @@
       <c r="A179" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B179" s="57">
+      <c r="B179" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C179" s="22">
@@ -6425,7 +6467,7 @@
       <c r="A180" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B180" s="57">
+      <c r="B180" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C180" s="22">
@@ -6439,7 +6481,7 @@
       <c r="A181" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B181" s="57">
+      <c r="B181" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C181" s="22">
@@ -6453,7 +6495,7 @@
       <c r="A182" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B182" s="57">
+      <c r="B182" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C182" s="22">
@@ -6464,7 +6506,7 @@
       <c r="A183" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B183" s="57">
+      <c r="B183" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C183" s="22">
@@ -6478,7 +6520,7 @@
       <c r="A184" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B184" s="57">
+      <c r="B184" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C184" s="22">
@@ -6492,7 +6534,7 @@
       <c r="A185" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="B185" s="57">
+      <c r="B185" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C185" s="22">
@@ -6503,7 +6545,7 @@
       <c r="A186" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="B186" s="57">
+      <c r="B186" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C186" s="22">
@@ -6514,7 +6556,7 @@
       <c r="A187" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B187" s="57">
+      <c r="B187" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C187" s="22">
@@ -6525,7 +6567,7 @@
       <c r="A188" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="B188" s="57">
+      <c r="B188" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C188" s="22">
@@ -6539,7 +6581,7 @@
       <c r="A189" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B189" s="57">
+      <c r="B189" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C189" s="33">
@@ -6553,7 +6595,7 @@
       <c r="A190" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B190" s="57">
+      <c r="B190" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C190" s="22">
@@ -6567,7 +6609,7 @@
       <c r="A191" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="B191" s="57">
+      <c r="B191" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C191" s="33">
@@ -6584,7 +6626,7 @@
       <c r="A192" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B192" s="57">
+      <c r="B192" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C192" s="22">
@@ -6598,7 +6640,7 @@
       <c r="A193" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="B193" s="57">
+      <c r="B193" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C193" s="22">
@@ -6612,7 +6654,7 @@
       <c r="A194" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B194" s="57">
+      <c r="B194" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C194" s="22">
@@ -6623,7 +6665,7 @@
       <c r="A195" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="B195" s="57">
+      <c r="B195" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C195" s="33">
@@ -6640,7 +6682,7 @@
       <c r="A196" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="B196" s="57">
+      <c r="B196" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C196" s="22">
@@ -6654,7 +6696,7 @@
       <c r="A197" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="B197" s="57">
+      <c r="B197" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C197" s="22">
@@ -6665,7 +6707,7 @@
       <c r="A198" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B198" s="57">
+      <c r="B198" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C198" s="22">
@@ -6679,7 +6721,7 @@
       <c r="A199" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="B199" s="57">
+      <c r="B199" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C199" s="22">
@@ -6690,7 +6732,7 @@
       <c r="A200" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="B200" s="57">
+      <c r="B200" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C200" s="22">
@@ -6701,7 +6743,7 @@
       <c r="A201" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="B201" s="57">
+      <c r="B201" s="56">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C201" s="22" t="s">
@@ -6869,7 +6911,7 @@
       <c r="C214" s="2">
         <v>3</v>
       </c>
-      <c r="D214" s="51" t="s">
+      <c r="D214" s="50" t="s">
         <v>865</v>
       </c>
     </row>
@@ -6888,7 +6930,7 @@
       </c>
     </row>
     <row r="216" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A216" s="52" t="s">
+      <c r="A216" s="51" t="s">
         <v>908</v>
       </c>
       <c r="B216" s="4" t="s">
@@ -6897,7 +6939,7 @@
       <c r="C216" s="31">
         <v>6</v>
       </c>
-      <c r="D216" s="53" t="s">
+      <c r="D216" s="52" t="s">
         <v>907</v>
       </c>
     </row>
@@ -6907,8 +6949,8 @@
       <c r="F217" s="31"/>
     </row>
   </sheetData>
-  <sortState ref="A40:D51">
-    <sortCondition descending="1" ref="B40:B51"/>
+  <sortState ref="A4:D37">
+    <sortCondition descending="1" ref="B4:B37"/>
   </sortState>
   <mergeCells count="10">
     <mergeCell ref="B1:D1"/>
@@ -7306,13 +7348,13 @@
       <c r="B2" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="53" t="s">
         <v>603</v>
       </c>
       <c r="F2" s="29" t="s">
@@ -7353,13 +7395,13 @@
       <c r="C3" s="32" t="s">
         <v>477</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="54" t="s">
         <v>607</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="54" t="s">
         <v>606</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="54" t="s">
         <v>605</v>
       </c>
       <c r="G3" s="32" t="s">
@@ -7394,19 +7436,19 @@
       <c r="B4" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>609</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="53" t="s">
         <v>608</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>925</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="53" t="s">
         <v>915</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="53" t="s">
         <v>916</v>
       </c>
       <c r="H4" s="29" t="s">
@@ -7441,10 +7483,10 @@
       <c r="C5" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="53" t="s">
         <v>917</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>918</v>
       </c>
       <c r="F5" s="29" t="s">
@@ -7482,19 +7524,19 @@
       <c r="B6" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>919</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>920</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>921</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="54" t="s">
         <v>922</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="54" t="s">
         <v>923</v>
       </c>
       <c r="H6" s="29" t="s">
@@ -7526,19 +7568,19 @@
       <c r="B7" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>919</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>920</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="53" t="s">
         <v>922</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="53" t="s">
         <v>926</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="53" t="s">
         <v>662</v>
       </c>
       <c r="H7" s="29" t="s">
@@ -7570,10 +7612,10 @@
       <c r="B8" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>639</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>877</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -7614,19 +7656,19 @@
       <c r="B9" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="53" t="s">
         <v>636</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="53" t="s">
         <v>609</v>
       </c>
-      <c r="G9" s="54" t="s">
+      <c r="G9" s="53" t="s">
         <v>635</v>
       </c>
       <c r="H9" s="29" t="s">
@@ -7661,16 +7703,16 @@
       <c r="C10" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="53" t="s">
         <v>649</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="53" t="s">
         <v>459</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="53" t="s">
         <v>648</v>
       </c>
       <c r="H10" s="29" t="s">
@@ -7702,19 +7744,19 @@
       <c r="B11" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>651</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>652</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="53" t="s">
         <v>653</v>
       </c>
-      <c r="F11" s="54" t="s">
+      <c r="F11" s="53" t="s">
         <v>654</v>
       </c>
-      <c r="G11" s="54" t="s">
+      <c r="G11" s="53" t="s">
         <v>655</v>
       </c>
       <c r="H11" s="29" t="s">
@@ -7746,19 +7788,19 @@
       <c r="B12" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>658</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="53" t="s">
         <v>659</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="53" t="s">
         <v>660</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="53" t="s">
         <v>661</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="53" t="s">
         <v>662</v>
       </c>
       <c r="H12" s="29" t="s">
@@ -7793,16 +7835,16 @@
       <c r="C13" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="53" t="s">
         <v>827</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="53" t="s">
         <v>820</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="53" t="s">
         <v>927</v>
       </c>
-      <c r="G13" s="54" t="s">
+      <c r="G13" s="53" t="s">
         <v>821</v>
       </c>
       <c r="H13" s="29" t="s">
@@ -7834,19 +7876,19 @@
       <c r="B14" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="53" t="s">
         <v>638</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>639</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="53" t="s">
         <v>640</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="53" t="s">
         <v>591</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="53" t="s">
         <v>641</v>
       </c>
       <c r="H14" s="29" t="s">
@@ -7878,19 +7920,19 @@
       <c r="B15" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="53" t="s">
         <v>827</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="53" t="s">
         <v>928</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="53" t="s">
         <v>929</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="53" t="s">
         <v>930</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="53" t="s">
         <v>931</v>
       </c>
       <c r="H15" s="29" t="s">
@@ -7922,25 +7964,25 @@
       <c r="B16" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>692</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="53" t="s">
         <v>693</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="53" t="s">
         <v>690</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="53" t="s">
         <v>423</v>
       </c>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="53" t="s">
         <v>691</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>597</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="48" t="s">
         <v>911</v>
       </c>
       <c r="J16" s="29" t="s">
@@ -7966,25 +8008,25 @@
       <c r="B17" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="54" t="s">
         <v>651</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="54" t="s">
         <v>823</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="54" t="s">
         <v>824</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="54" t="s">
         <v>459</v>
       </c>
-      <c r="G17" s="55" t="s">
+      <c r="G17" s="54" t="s">
         <v>648</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>597</v>
       </c>
-      <c r="I17" s="49" t="s">
+      <c r="I17" s="48" t="s">
         <v>825</v>
       </c>
       <c r="J17" s="29" t="s">
@@ -8010,19 +8052,19 @@
       <c r="B18" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="53" t="s">
         <v>651</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="53" t="s">
         <v>652</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="53" t="s">
         <v>649</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="53" t="s">
         <v>655</v>
       </c>
       <c r="H18" s="29" t="s">
@@ -8057,16 +8099,16 @@
       <c r="C19" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="53" t="s">
         <v>932</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="53" t="s">
         <v>933</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="F19" s="53" t="s">
         <v>605</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="53" t="s">
         <v>724</v>
       </c>
       <c r="H19" s="29" t="s">
@@ -8098,19 +8140,19 @@
       <c r="B20" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="54" t="s">
         <v>920</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="54" t="s">
         <v>636</v>
       </c>
-      <c r="F20" s="54" t="s">
+      <c r="F20" s="53" t="s">
         <v>732</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="53" t="s">
         <v>877</v>
       </c>
       <c r="H20" s="29" t="s">
@@ -8145,16 +8187,16 @@
       <c r="C21" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="53" t="s">
         <v>662</v>
       </c>
       <c r="H21" s="29" t="s">
@@ -8186,19 +8228,19 @@
       <c r="B22" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="54" t="s">
         <v>870</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="54" t="s">
         <v>871</v>
       </c>
-      <c r="F22" s="55" t="s">
+      <c r="F22" s="54" t="s">
         <v>872</v>
       </c>
-      <c r="G22" s="55" t="s">
+      <c r="G22" s="54" t="s">
         <v>873</v>
       </c>
       <c r="H22" s="29" t="s">
@@ -8230,19 +8272,19 @@
       <c r="B23" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="54" t="s">
         <v>639</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="54" t="s">
         <v>880</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="54" t="s">
         <v>439</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F23" s="54" t="s">
         <v>934</v>
       </c>
-      <c r="G23" s="55" t="s">
+      <c r="G23" s="54" t="s">
         <v>935</v>
       </c>
       <c r="H23" s="29" t="s">
@@ -8274,19 +8316,19 @@
       <c r="B24" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="54" t="s">
         <v>936</v>
       </c>
-      <c r="F24" s="55" t="s">
+      <c r="F24" s="54" t="s">
         <v>661</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="48" t="s">
         <v>477</v>
       </c>
       <c r="H24" s="29" t="s">
@@ -8313,36 +8355,36 @@
     </row>
     <row r="25" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
     </row>
     <row r="26" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>699</v>
       </c>
       <c r="B26" s="20"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
       <c r="O26" s="31"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="31"/>
@@ -8357,13 +8399,13 @@
       <c r="B27" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="54" t="s">
         <v>601</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="54" t="s">
         <v>602</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="54" t="s">
         <v>603</v>
       </c>
       <c r="F27" s="29" t="s">
@@ -8372,7 +8414,7 @@
       <c r="G27" s="29" t="s">
         <v>595</v>
       </c>
-      <c r="H27" s="55" t="s">
+      <c r="H27" s="54" t="s">
         <v>700</v>
       </c>
       <c r="I27" s="29" t="s">
@@ -8394,12 +8436,12 @@
         <v>600</v>
       </c>
       <c r="O27" s="31"/>
-      <c r="P27" s="62" t="s">
+      <c r="P27" s="64" t="s">
         <v>819</v>
       </c>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="64"/>
+      <c r="S27" s="64"/>
       <c r="T27" s="31"/>
     </row>
     <row r="28" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -8409,10 +8451,10 @@
       <c r="B28" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="54" t="s">
         <v>920</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="54" t="s">
         <v>922</v>
       </c>
       <c r="E28" s="29" t="s">
@@ -8424,7 +8466,7 @@
       <c r="G28" s="29" t="s">
         <v>595</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="54" t="s">
         <v>427</v>
       </c>
       <c r="I28" s="29" t="s">
@@ -8459,22 +8501,22 @@
       <c r="B29" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="54" t="s">
         <v>662</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="54" t="s">
         <v>937</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="54" t="s">
         <v>938</v>
       </c>
-      <c r="F29" s="55" t="s">
+      <c r="F29" s="54" t="s">
         <v>939</v>
       </c>
-      <c r="G29" s="55" t="s">
+      <c r="G29" s="54" t="s">
         <v>940</v>
       </c>
-      <c r="H29" s="55" t="s">
+      <c r="H29" s="54" t="s">
         <v>713</v>
       </c>
       <c r="I29" s="29" t="s">
@@ -8509,22 +8551,22 @@
       <c r="B30" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="54" t="s">
         <v>941</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="54" t="s">
         <v>942</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="54" t="s">
         <v>943</v>
       </c>
-      <c r="F30" s="55" t="s">
+      <c r="F30" s="54" t="s">
         <v>944</v>
       </c>
-      <c r="G30" s="55" t="s">
+      <c r="G30" s="54" t="s">
         <v>945</v>
       </c>
-      <c r="H30" s="55" t="s">
+      <c r="H30" s="54" t="s">
         <v>946</v>
       </c>
       <c r="I30" s="29" t="s">
@@ -8559,22 +8601,22 @@
       <c r="B31" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="54" t="s">
         <v>925</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D31" s="54" t="s">
         <v>636</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="54" t="s">
         <v>639</v>
       </c>
-      <c r="F31" s="55" t="s">
+      <c r="F31" s="54" t="s">
         <v>732</v>
       </c>
-      <c r="G31" s="55" t="s">
+      <c r="G31" s="54" t="s">
         <v>635</v>
       </c>
-      <c r="H31" s="55" t="s">
+      <c r="H31" s="54" t="s">
         <v>641</v>
       </c>
       <c r="I31" s="29" t="s">
@@ -8603,22 +8645,22 @@
       <c r="B32" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="54" t="s">
         <v>919</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="54" t="s">
         <v>920</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="54" t="s">
         <v>922</v>
       </c>
-      <c r="F32" s="55" t="s">
+      <c r="F32" s="54" t="s">
         <v>638</v>
       </c>
-      <c r="G32" s="55" t="s">
+      <c r="G32" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="H32" s="55" t="s">
+      <c r="H32" s="54" t="s">
         <v>744</v>
       </c>
       <c r="I32" s="29" t="s">
@@ -8647,22 +8689,22 @@
       <c r="B33" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="53" t="s">
         <v>827</v>
       </c>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="54" t="s">
         <v>938</v>
       </c>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="54" t="s">
         <v>947</v>
       </c>
-      <c r="F33" s="54" t="s">
+      <c r="F33" s="53" t="s">
         <v>927</v>
       </c>
-      <c r="G33" s="54" t="s">
+      <c r="G33" s="53" t="s">
         <v>821</v>
       </c>
-      <c r="H33" s="54" t="s">
+      <c r="H33" s="53" t="s">
         <v>820</v>
       </c>
       <c r="I33" s="29" t="s">
@@ -8740,7 +8782,7 @@
       <c r="L36" s="4" t="s">
         <v>809</v>
       </c>
-      <c r="M36" s="49" t="s">
+      <c r="M36" s="48" t="s">
         <v>808</v>
       </c>
       <c r="N36" s="1" t="s">
@@ -9039,7 +9081,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="49" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -9211,7 +9253,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="49" t="s">
         <v>503</v>
       </c>
       <c r="B13" t="s">
@@ -9254,7 +9296,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
@@ -9309,10 +9351,10 @@
       <c r="D17" t="s">
         <v>349</v>
       </c>
-      <c r="F17" s="64">
+      <c r="F17" s="66">
         <v>23.6</v>
       </c>
-      <c r="G17" s="63">
+      <c r="G17" s="65">
         <v>45</v>
       </c>
     </row>
@@ -9329,8 +9371,8 @@
       <c r="D18" t="s">
         <v>478</v>
       </c>
-      <c r="F18" s="64"/>
-      <c r="G18" s="63"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="65"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -9565,7 +9607,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -10322,10 +10364,10 @@
       <c r="E18" t="s">
         <v>765</v>
       </c>
-      <c r="F18" s="62">
+      <c r="F18" s="64">
         <v>3.5</v>
       </c>
-      <c r="G18" s="62">
+      <c r="G18" s="64">
         <v>3.5</v>
       </c>
     </row>
@@ -10339,8 +10381,8 @@
       <c r="E19" t="s">
         <v>766</v>
       </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">

</xml_diff>